<commit_message>
Updated input data document to test
</commit_message>
<xml_diff>
--- a/PriorTool_Input_Data.xlsx
+++ b/PriorTool_Input_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bencahill/Documents/python_progs/Prioritising_Tool/PriorTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3CC79C-4018-BB48-9285-FECC3346170C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EABF672-0F00-A941-8BA7-B37B69DBB9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{A8BEBEA9-D1E6-634C-884B-3ACC2F953EB0}"/>
   </bookViews>
@@ -36,15 +36,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>ACTIVITY_TYPE_1</t>
   </si>
   <si>
-    <t>QUESTION_1</t>
-  </si>
-  <si>
-    <t>QUESTION_1_TYPE</t>
+    <t>ACTIVITY_TYPE_2</t>
+  </si>
+  <si>
+    <t>ACTIVITY_TYPE_3</t>
+  </si>
+  <si>
+    <t>Is there Food?</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>How much food is there?</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>QUESTION</t>
+  </si>
+  <si>
+    <t>QUESTION_TYPE</t>
   </si>
 </sst>
 </file>
@@ -416,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76784108-58B2-6945-B52F-A78989885E15}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,19 +447,54 @@
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>